<commit_message>
added outbreak codes to two clinical samples
</commit_message>
<xml_diff>
--- a/datasets/Listeria_monocytogenes_1408MLGX6-3WGS.xlsx
+++ b/datasets/Listeria_monocytogenes_1408MLGX6-3WGS.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="177">
   <si>
     <t>Organism</t>
   </si>
@@ -1008,7 +1008,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1877,7 +1877,9 @@
       <c r="D36" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E36" s="15"/>
+      <c r="E36" s="15" t="s">
+        <v>108</v>
+      </c>
       <c r="F36" s="14" t="s">
         <v>108</v>
       </c>
@@ -1929,7 +1931,9 @@
       <c r="D38" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="E38" s="15"/>
+      <c r="E38" s="15" t="s">
+        <v>108</v>
+      </c>
       <c r="F38" s="14" t="s">
         <v>108</v>
       </c>

</xml_diff>

<commit_message>
downloads tree and copies over spreadsheet now
</commit_message>
<xml_diff>
--- a/datasets/Listeria_monocytogenes_1408MLGX6-3WGS.xlsx
+++ b/datasets/Listeria_monocytogenes_1408MLGX6-3WGS.xlsx
@@ -391,24 +391,6 @@
     <t>0efd95ce1e936dd239922f5f90081b6a4ecdf56f238229159446c40b64ec42dc</t>
   </si>
   <si>
-    <t>15e122d14b8254173da26748ce10dd3b975956f853baf1487b5abd07e34af1ae</t>
-  </si>
-  <si>
-    <t>4b7c11548c9b634e096adfd566eff1a57452bfe1283ea4c87aaf33342094308c</t>
-  </si>
-  <si>
-    <t>8599e37dcfa4300e51cd60d21b9111306c6d1a0d25338ffe6cfa8406c958954d</t>
-  </si>
-  <si>
-    <t>01edf3fbf763f7b29e11c7ba82577c6582baa28d71bca929f8986f6d9e670e64</t>
-  </si>
-  <si>
-    <t>cff5089077fcad2612b06b1e04c3970fea559f1e17d1a31b6ae9ebc88100deba</t>
-  </si>
-  <si>
-    <t>2e0fc66405ba7b64b7655d1c93d29dc8bf27d48e207c280867594d84cbf1f187</t>
-  </si>
-  <si>
     <t>977eca15028a86972d45959801f37e06bcd9c4d737493bb22d2cff2ca5c0d4d2</t>
   </si>
   <si>
@@ -421,12 +403,6 @@
     <t>a4bcd49b45d7ad5295bbe097874526ff2813bdd2d8f07a1f4738a4f06d320f47</t>
   </si>
   <si>
-    <t>e9fec1f1979bd2af0059b8b65b59c1ae98cfdd051aaf3915075167d708c29bff</t>
-  </si>
-  <si>
-    <t>5929e36fbfc58de4d358b1bb9adca26c27d12c78faca198e69bcc7fc868c1869</t>
-  </si>
-  <si>
     <t>0b06c23ef4414922849dc2396bc79c82f445cb3b2c62e720dff98d6ceddb9bdd</t>
   </si>
   <si>
@@ -439,12 +415,6 @@
     <t>94e9da477bfa6c02ca22ed7fcc239c8fae93c363a6ca9eeffcfa69d7b88e1487</t>
   </si>
   <si>
-    <t>99a8e4b8bee42f25ed66ff1f0a6fc831686fde224ea33321939e43ba1f2f8dc8</t>
-  </si>
-  <si>
-    <t>20e55ffe8f6f1416b5021e8cda79b2c55396f3b33772cceaad8c5ebc6417dffe</t>
-  </si>
-  <si>
     <t>db7b609d66e9a253f4ad54fcc4f62b578562f4368dca56658ecae14effd7811c</t>
   </si>
   <si>
@@ -463,84 +433,18 @@
     <t>0a3528a4e2aa3a2aade719858ef702dbba459b1c7a7bd49d7c504cd20f2b1b71</t>
   </si>
   <si>
-    <t>971027fb25f15dbfba5c8033afe0876065e9a9c2a2df868c80e4e9d6ebdfdc7f</t>
-  </si>
-  <si>
-    <t>a3437b7c129affd4d9a2bc18990a1e2f8c1a7b446856dca87eb61afc29b5a1ec</t>
-  </si>
-  <si>
-    <t>66095b1a6aefce03fccdcb0f189275ac81034dec93516363331aabf277b0b7b2</t>
-  </si>
-  <si>
-    <t>cd27f22e033916b64b14ccce9432bbf9bd6356ccf6db7546a29932f8d41cbe8d</t>
-  </si>
-  <si>
     <t>8acda8ca5472afae4de08f428bf03bc8cbb432218cbe70eeed57d2d194ad7173</t>
   </si>
   <si>
     <t>5cab244a209484464d815e66e35bc351fa0f1df7d60f3d316c883f980b2b0a02</t>
   </si>
   <si>
-    <t>5bc7e3a960214af95defb5f394694b5d3d9a6d78ada650f0080089b83990cc57</t>
-  </si>
-  <si>
-    <t>197530bf9091c71fb25fffb065035ccef04325380c4ebe3bd176cc9e1a79f1a8</t>
-  </si>
-  <si>
-    <t>81a89038975b6dd892a69f279d9aea0f0fac1fa15598b8bca7d7555ff874bbe5</t>
-  </si>
-  <si>
-    <t>808b4c08ecc83acf91e6876d3f85f8c9a7248f50412de8338dcfaa34b659d86b</t>
-  </si>
-  <si>
-    <t>9da7c52e8c519a516fd02ee25c9c70160863f5705de221e53039c387d3ebc978</t>
-  </si>
-  <si>
-    <t>3d5fecc0b8b00133e2991adfe59f1c56e0e1cddd9cc82dc5a33f6c4076db4375</t>
-  </si>
-  <si>
-    <t>6683ea50c9d03795dedfeb6195bd320331345780da296a6a06c973de19565698</t>
-  </si>
-  <si>
-    <t>4dfe0c507369971ab806f380286d98f92950d268b8479c420181efd14aa50932</t>
-  </si>
-  <si>
     <t>63ec4512f73e24b45b1ad435b6ab4ea9e4c6720a0aa0b2a77fa25b88c81dd3ca</t>
   </si>
   <si>
     <t>28ffce5aa3f8b613a93e0baa663bea84d3fb3030580ad80690d44443b5cc7a49</t>
   </si>
   <si>
-    <t>774f96efeeb98d4ec30b192622d69338d9798ef7d478226eb8ac2f1bceefef70</t>
-  </si>
-  <si>
-    <t>f1fce2bb09bc9a860177fc32c87a00cba72a3e8b2216cb2281fc455053866408</t>
-  </si>
-  <si>
-    <t>661a68e0ce9c7671d5236aee7f8c01d94851248ddc798c0afe2e39d370cc1289</t>
-  </si>
-  <si>
-    <t>1ae71a70ec8dbce53a1fb70163633a99bc4abcf7d1f21a40ff5c5225937611a0</t>
-  </si>
-  <si>
-    <t>ceb299f4eefdaf45b1a603cade79d71c1c0b6c1a256a432358739c7b60d22fd1</t>
-  </si>
-  <si>
-    <t>53660f0710d260f9ebfaf47dcebd66b9c3d51c58d089011a57e0f160534b1864</t>
-  </si>
-  <si>
-    <t>da2d694a66cbb47477f54c23cc433b55406fd4eaf2aece6e2420f832f2e0376e</t>
-  </si>
-  <si>
-    <t>3e84133e1b872c590b0b6c81434630b32c93dafcf17f48f918a7768921fbee13</t>
-  </si>
-  <si>
-    <t>8bd255e69eb3d304c99922562e5b56e9f484d9bec8a3896c40cca799064c3475</t>
-  </si>
-  <si>
-    <t>bcc216ba76852418eb5de9077126577c95e107167be8416bb59e514fd97040b2</t>
-  </si>
-  <si>
     <t>6083e21eb921ca0ce0648d27924878b3bcfb719a2ecd3a334bddb83940f6ae3c</t>
   </si>
   <si>
@@ -553,25 +457,121 @@
     <t>908a57d326b40ac34f3aec3c7829651927724e77933a014fa39d72c0770a1dca</t>
   </si>
   <si>
-    <t>21f9479a315a749d3f9bb88ac750b86bad4e75f92d2e7a813475e5a3be1cdd67</t>
-  </si>
-  <si>
-    <t>f11b2383e3efa59325acf990840545dc444817adc14e08421f4ff628410dddb1</t>
-  </si>
-  <si>
-    <t>3931b8ecaf099558ac0b4f327ef24ae64caa697950094213ef55c08045384249</t>
-  </si>
-  <si>
-    <t>4cf19c2ecccbc1b8ae1156d936c32e727da963263927e6422fc6d197eb553cba</t>
-  </si>
-  <si>
-    <t>1540a600a617634e9e8bede6b9c4b41a57756186ab62178b2507e8090cb8ad2b</t>
-  </si>
-  <si>
-    <t>e1560a8800930276c68b155ca0eec46a3dc9bd45533abe037eb9813f36c75b45</t>
-  </si>
-  <si>
     <t>d531614e1b1ba70261a6840d0ca422df90a963d6b9b696d635b8bbcc05cc07af</t>
+  </si>
+  <si>
+    <t>8700b6087a2c36bcc2ca8e370fb340a0a749567ff6f158eae963067f781861cf</t>
+  </si>
+  <si>
+    <t>748505e11bdcd90d49ff2a2e784724a231668b1009801d7af53ff2cc80ce2084</t>
+  </si>
+  <si>
+    <t>0af517b6258816dc42aa6a94cfda3bbd5a27ca990499f05fd26b33f721aa3cd3</t>
+  </si>
+  <si>
+    <t>170b447f26139c2d9dfe60065eeba7faca76908e36932905924c8435805aa7bc</t>
+  </si>
+  <si>
+    <t>42062c61614a5cedec3de285e91327fad8cfab5db4d8dbd4cee512bb72353c54</t>
+  </si>
+  <si>
+    <t>dea029782dfec718104252c3470ff7de7a401a433e011570f1abb99bb3a19b1c</t>
+  </si>
+  <si>
+    <t>e48a1af5bec79f2bca3fa72790abc4265f049de0d809a074643667464de30230</t>
+  </si>
+  <si>
+    <t>884ae69d5a14b57dd1ee47ac9be159f8ce597255148b6c9f6c323a18144f2907</t>
+  </si>
+  <si>
+    <t>c43c41991ad8ed40ffcebbde36dc9011f471dea643fc8f715621a2e336095bf5</t>
+  </si>
+  <si>
+    <t>4d12ed7e34b2456b8444dd71287cbb83b9c45bd18dc23627af0fbb6014ac0fca</t>
+  </si>
+  <si>
+    <t>4ba5b7d004471815c7e9096e93e6d94053b89aad5b20305ac0df872ec265e06d</t>
+  </si>
+  <si>
+    <t>20f5e00dd444a398f773b5bc66e9fd81be7e9f500b7baf9bfd31796f411ae0f3</t>
+  </si>
+  <si>
+    <t>7c26b121c6efa3bcba8f1e0a2ca121e83104814d34cb99c5c4890b5c22ec37a8</t>
+  </si>
+  <si>
+    <t>97490a7ce0716ca6003c5ee3fd48f348611deed9f23b7c6660d6e04610d60019</t>
+  </si>
+  <si>
+    <t>03893d64d118c381d0a440bfb9a1647e719093ca68fa4b56590a1c3ae7bd8fc2</t>
+  </si>
+  <si>
+    <t>bc944255904d5ed0fa81d5aa53d83331a1119e759dac0c7f7a091756a6bb788d</t>
+  </si>
+  <si>
+    <t>c1b53f6e3c754c116983d3a46a8a4d10cd2fcdf1163ff83faaa97ecfa77a3b23</t>
+  </si>
+  <si>
+    <t>f57d4a8d677997019522664785c11c338147cd9ca83ae2ec0ddefdd81f85bc03</t>
+  </si>
+  <si>
+    <t>530cb2a004bd3d2b3fa390e2ffd92e55c4da3ce773390e74ab3e70028f37de94</t>
+  </si>
+  <si>
+    <t>6cff309484738b5051db57d2d8617d467e4463e43370de951e3f74004dda4b03</t>
+  </si>
+  <si>
+    <t>2ea5cf8158f1973bbf2427c03b083e8b0936329f262810e824cf5b278269cd07</t>
+  </si>
+  <si>
+    <t>f4a7334433ad5fa9354d9b82ad3234a319ee731530d2c92b67e1fdd41157eb2a</t>
+  </si>
+  <si>
+    <t>d9a377d64605d955ae85118f5572de13635004c3d377f5366d86236337318d0c</t>
+  </si>
+  <si>
+    <t>9ba0910aad655e05c2915148efcde2b03a6e31251987b0aa79611bcc890e6211</t>
+  </si>
+  <si>
+    <t>f092fda1f48a5f496b51971a907b3069716eb2bbf5f96d7aa2ae2a4932696fdb</t>
+  </si>
+  <si>
+    <t>eb435d21eb8d5c47e882e010ffb5fdaf14241ad647ffb3be78cc44c3b0e1a0f6</t>
+  </si>
+  <si>
+    <t>bc4e509d9a7b67ba52885a79b89926d49e3ceba1ab3043b1d7cd2eb0c744054c</t>
+  </si>
+  <si>
+    <t>e04208ebe9a5a3473c9506211964cc55040ed366b8112cc0ce9dd782529e6e3b</t>
+  </si>
+  <si>
+    <t>b370ed5e82f48714225102dfa38f252a93c5eff4bae2c7b03eb980e34d2b22f0</t>
+  </si>
+  <si>
+    <t>509e4a7a36c8e8e28d9b9664d3a5c9a1a0be02ba3f056a52d05ad65acaba4203</t>
+  </si>
+  <si>
+    <t>10fb5acccaa8fc22871797095c9b56b9beac147c6cccb79a6e4bc0548007ff88</t>
+  </si>
+  <si>
+    <t>9ac124aedaac05f7751ab96a77e2298090417aae085ff9ee35aa797823520574</t>
+  </si>
+  <si>
+    <t>8fa5ae2ef989472927cc68b0171e7e601206d71649bc71696d112140ac840021</t>
+  </si>
+  <si>
+    <t>a2ee8c969091a990cedbe247c9e7cf2da9c1921eda0bbffb892e52901d78220b</t>
+  </si>
+  <si>
+    <t>e2cdd58cad197564206bac754e893887161b7cc941231c8b731655f2223beb86</t>
+  </si>
+  <si>
+    <t>64d6c5006ddb3f567c44adf716669c3c15ac876ba7c7d8c31cbf2c7049936dd6</t>
+  </si>
+  <si>
+    <t>651ceeb1bbb975c53f3f96b4eab50160b593dd2c277e6b07e59343018b645124</t>
+  </si>
+  <si>
+    <t>01ce691d4a9dbfdc5929071f9ce2387215e62253cd76eb1a96533271bcdf6438</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9:J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,13 +1131,13 @@
         <v>1</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>176</v>
+        <v>138</v>
       </c>
       <c r="I9" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="J9" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1190,10 +1190,10 @@
       </c>
       <c r="H11" s="12"/>
       <c r="I11" t="s">
-        <v>116</v>
+        <v>165</v>
       </c>
       <c r="J11" t="s">
-        <v>117</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1218,10 +1218,10 @@
       </c>
       <c r="H12" s="12"/>
       <c r="I12" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="J12" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1246,10 +1246,10 @@
       </c>
       <c r="H13" s="12"/>
       <c r="I13" t="s">
-        <v>120</v>
+        <v>145</v>
       </c>
       <c r="J13" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1274,10 +1274,10 @@
       </c>
       <c r="H14" s="12"/>
       <c r="I14" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="J14" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1302,10 +1302,10 @@
       </c>
       <c r="H15" s="12"/>
       <c r="I15" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="J15" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1330,10 +1330,10 @@
       </c>
       <c r="H16" s="12"/>
       <c r="I16" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="J16" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1358,10 +1358,10 @@
       </c>
       <c r="H17" s="12"/>
       <c r="I17" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="J17" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1386,10 +1386,10 @@
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="16" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="J18" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1414,10 +1414,10 @@
       </c>
       <c r="H19" s="12"/>
       <c r="I19" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="J19" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1442,10 +1442,10 @@
       </c>
       <c r="H20" s="12"/>
       <c r="I20" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="J20" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1470,10 +1470,10 @@
       </c>
       <c r="H21" s="12"/>
       <c r="I21" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="J21" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1498,10 +1498,10 @@
       </c>
       <c r="H22" s="12"/>
       <c r="I22" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="J22" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1526,10 +1526,10 @@
       </c>
       <c r="H23" s="12"/>
       <c r="I23" t="s">
+        <v>139</v>
+      </c>
+      <c r="J23" t="s">
         <v>140</v>
-      </c>
-      <c r="J23" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1554,10 +1554,10 @@
       </c>
       <c r="H24" s="12"/>
       <c r="I24" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="J24" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1582,10 +1582,10 @@
       </c>
       <c r="H25" s="12"/>
       <c r="I25" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="J25" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1610,10 +1610,10 @@
       </c>
       <c r="H26" s="12"/>
       <c r="I26" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="J26" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1638,10 +1638,10 @@
       </c>
       <c r="H27" s="12"/>
       <c r="I27" t="s">
-        <v>148</v>
+        <v>167</v>
       </c>
       <c r="J27" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1666,10 +1666,10 @@
       </c>
       <c r="H28" s="12"/>
       <c r="I28" t="s">
-        <v>150</v>
+        <v>169</v>
       </c>
       <c r="J28" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1694,10 +1694,10 @@
       </c>
       <c r="H29" s="12"/>
       <c r="I29" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="J29" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1722,10 +1722,10 @@
       </c>
       <c r="H30" s="12"/>
       <c r="I30" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="J30" t="s">
-        <v>155</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1750,10 +1750,10 @@
       </c>
       <c r="H31" s="12"/>
       <c r="I31" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="J31" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1778,10 +1778,10 @@
       </c>
       <c r="H32" s="12"/>
       <c r="I32" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="J32" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1806,10 +1806,10 @@
       </c>
       <c r="H33" s="12"/>
       <c r="I33" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="J33" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1834,10 +1834,10 @@
       </c>
       <c r="H34" s="12"/>
       <c r="I34" t="s">
-        <v>162</v>
+        <v>173</v>
       </c>
       <c r="J34" s="16" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1860,10 +1860,10 @@
       </c>
       <c r="H35" s="12"/>
       <c r="I35" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="J35" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1888,10 +1888,10 @@
       </c>
       <c r="H36" s="12"/>
       <c r="I36" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
       <c r="J36" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1914,10 +1914,10 @@
       </c>
       <c r="H37" s="12"/>
       <c r="I37" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="J37" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1942,10 +1942,10 @@
       </c>
       <c r="H38" s="12"/>
       <c r="I38" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="J38" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
@@ -1968,10 +1968,10 @@
       </c>
       <c r="H39" s="12"/>
       <c r="I39" t="s">
-        <v>172</v>
+        <v>147</v>
       </c>
       <c r="J39" t="s">
-        <v>173</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
filled in all values as best I could
</commit_message>
<xml_diff>
--- a/datasets/Listeria_monocytogenes_1408MLGX6-3WGS.xlsx
+++ b/datasets/Listeria_monocytogenes_1408MLGX6-3WGS.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="179">
   <si>
     <t>Organism</t>
   </si>
@@ -572,6 +572,12 @@
   </si>
   <si>
     <t>01ce691d4a9dbfdc5929071f9ce2387215e62253cd76eb1a96533271bcdf6438</t>
+  </si>
+  <si>
+    <t>outgroup</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9:J39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1153,9 @@
       <c r="B10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="12"/>
+      <c r="C10" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D10" s="12" t="s">
         <v>19</v>
       </c>
@@ -1160,7 +1168,9 @@
       <c r="G10" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I10" t="s">
         <v>114</v>
       </c>
@@ -1175,7 +1185,9 @@
       <c r="B11" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D11" s="12" t="s">
         <v>21</v>
       </c>
@@ -1188,7 +1200,9 @@
       <c r="G11" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H11" s="12"/>
+      <c r="H11" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I11" t="s">
         <v>165</v>
       </c>
@@ -1203,7 +1217,9 @@
       <c r="B12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="12"/>
+      <c r="C12" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D12" s="12" t="s">
         <v>23</v>
       </c>
@@ -1216,7 +1232,9 @@
       <c r="G12" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H12" s="12"/>
+      <c r="H12" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I12" t="s">
         <v>149</v>
       </c>
@@ -1231,7 +1249,9 @@
       <c r="B13" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="12"/>
+      <c r="C13" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D13" s="12" t="s">
         <v>25</v>
       </c>
@@ -1244,7 +1264,9 @@
       <c r="G13" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H13" s="12"/>
+      <c r="H13" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I13" t="s">
         <v>145</v>
       </c>
@@ -1259,7 +1281,9 @@
       <c r="B14" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D14" s="12" t="s">
         <v>27</v>
       </c>
@@ -1272,7 +1296,9 @@
       <c r="G14" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H14" s="12"/>
+      <c r="H14" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I14" t="s">
         <v>116</v>
       </c>
@@ -1287,7 +1313,9 @@
       <c r="B15" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="12"/>
+      <c r="C15" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D15" s="12" t="s">
         <v>29</v>
       </c>
@@ -1300,7 +1328,9 @@
       <c r="G15" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H15" s="12"/>
+      <c r="H15" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I15" t="s">
         <v>118</v>
       </c>
@@ -1315,7 +1345,9 @@
       <c r="B16" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D16" s="12" t="s">
         <v>31</v>
       </c>
@@ -1328,7 +1360,9 @@
       <c r="G16" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H16" s="12"/>
+      <c r="H16" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I16" t="s">
         <v>153</v>
       </c>
@@ -1343,7 +1377,9 @@
       <c r="B17" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="12"/>
+      <c r="C17" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D17" s="12" t="s">
         <v>33</v>
       </c>
@@ -1356,7 +1392,9 @@
       <c r="G17" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H17" s="12"/>
+      <c r="H17" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I17" t="s">
         <v>120</v>
       </c>
@@ -1371,7 +1409,9 @@
       <c r="B18" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="12"/>
+      <c r="C18" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D18" s="12" t="s">
         <v>35</v>
       </c>
@@ -1384,7 +1424,9 @@
       <c r="G18" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H18" s="12"/>
+      <c r="H18" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I18" s="16" t="s">
         <v>122</v>
       </c>
@@ -1399,7 +1441,9 @@
       <c r="B19" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="12"/>
+      <c r="C19" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D19" s="12" t="s">
         <v>37</v>
       </c>
@@ -1412,7 +1456,9 @@
       <c r="G19" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H19" s="12"/>
+      <c r="H19" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I19" t="s">
         <v>141</v>
       </c>
@@ -1427,7 +1473,9 @@
       <c r="B20" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D20" s="12" t="s">
         <v>39</v>
       </c>
@@ -1440,7 +1488,9 @@
       <c r="G20" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H20" s="12"/>
+      <c r="H20" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I20" t="s">
         <v>124</v>
       </c>
@@ -1455,7 +1505,9 @@
       <c r="B21" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D21" s="12" t="s">
         <v>41</v>
       </c>
@@ -1468,7 +1520,9 @@
       <c r="G21" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H21" s="12"/>
+      <c r="H21" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I21" t="s">
         <v>126</v>
       </c>
@@ -1483,7 +1537,9 @@
       <c r="B22" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C22" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D22" s="12" t="s">
         <v>43</v>
       </c>
@@ -1496,7 +1552,9 @@
       <c r="G22" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H22" s="12"/>
+      <c r="H22" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I22" t="s">
         <v>128</v>
       </c>
@@ -1511,7 +1569,9 @@
       <c r="B23" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D23" s="12" t="s">
         <v>45</v>
       </c>
@@ -1524,7 +1584,9 @@
       <c r="G23" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H23" s="12"/>
+      <c r="H23" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I23" t="s">
         <v>139</v>
       </c>
@@ -1539,7 +1601,9 @@
       <c r="B24" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D24" s="12" t="s">
         <v>47</v>
       </c>
@@ -1552,7 +1616,9 @@
       <c r="G24" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H24" s="12"/>
+      <c r="H24" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I24" t="s">
         <v>157</v>
       </c>
@@ -1567,7 +1633,9 @@
       <c r="B25" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D25" s="12" t="s">
         <v>49</v>
       </c>
@@ -1580,7 +1648,9 @@
       <c r="G25" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H25" s="12"/>
+      <c r="H25" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I25" t="s">
         <v>130</v>
       </c>
@@ -1595,7 +1665,9 @@
       <c r="B26" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="12"/>
+      <c r="C26" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D26" s="12" t="s">
         <v>51</v>
       </c>
@@ -1608,7 +1680,9 @@
       <c r="G26" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H26" s="12"/>
+      <c r="H26" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I26" t="s">
         <v>155</v>
       </c>
@@ -1623,7 +1697,9 @@
       <c r="B27" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="12"/>
+      <c r="C27" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D27" s="12" t="s">
         <v>53</v>
       </c>
@@ -1636,7 +1712,9 @@
       <c r="G27" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H27" s="12"/>
+      <c r="H27" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I27" t="s">
         <v>167</v>
       </c>
@@ -1651,7 +1729,9 @@
       <c r="B28" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="12"/>
+      <c r="C28" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D28" s="12" t="s">
         <v>55</v>
       </c>
@@ -1664,7 +1744,9 @@
       <c r="G28" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H28" s="12"/>
+      <c r="H28" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I28" t="s">
         <v>169</v>
       </c>
@@ -1679,7 +1761,9 @@
       <c r="B29" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D29" s="12" t="s">
         <v>57</v>
       </c>
@@ -1692,7 +1776,9 @@
       <c r="G29" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H29" s="12"/>
+      <c r="H29" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I29" t="s">
         <v>143</v>
       </c>
@@ -1707,7 +1793,9 @@
       <c r="B30" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C30" s="12"/>
+      <c r="C30" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D30" s="12" t="s">
         <v>59</v>
       </c>
@@ -1720,7 +1808,9 @@
       <c r="G30" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H30" s="12"/>
+      <c r="H30" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I30" t="s">
         <v>132</v>
       </c>
@@ -1735,7 +1825,9 @@
       <c r="B31" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D31" s="12" t="s">
         <v>61</v>
       </c>
@@ -1748,7 +1840,9 @@
       <c r="G31" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H31" s="12"/>
+      <c r="H31" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I31" t="s">
         <v>151</v>
       </c>
@@ -1763,7 +1857,9 @@
       <c r="B32" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D32" s="12" t="s">
         <v>63</v>
       </c>
@@ -1776,7 +1872,9 @@
       <c r="G32" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H32" s="12"/>
+      <c r="H32" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I32" t="s">
         <v>159</v>
       </c>
@@ -1791,7 +1889,9 @@
       <c r="B33" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="12"/>
+      <c r="C33" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D33" s="12" t="s">
         <v>65</v>
       </c>
@@ -1804,7 +1904,9 @@
       <c r="G33" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H33" s="12"/>
+      <c r="H33" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I33" t="s">
         <v>171</v>
       </c>
@@ -1819,7 +1921,9 @@
       <c r="B34" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D34" s="12" t="s">
         <v>67</v>
       </c>
@@ -1832,7 +1936,9 @@
       <c r="G34" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H34" s="12"/>
+      <c r="H34" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I34" t="s">
         <v>173</v>
       </c>
@@ -1847,18 +1953,24 @@
       <c r="B35" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="12"/>
+      <c r="C35" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D35" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="15"/>
+      <c r="E35" s="15" t="s">
+        <v>177</v>
+      </c>
       <c r="F35" s="14" t="s">
         <v>108</v>
       </c>
       <c r="G35" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H35" s="12"/>
+      <c r="H35" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I35" t="s">
         <v>161</v>
       </c>
@@ -1873,7 +1985,9 @@
       <c r="B36" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="12"/>
+      <c r="C36" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D36" s="12" t="s">
         <v>71</v>
       </c>
@@ -1886,7 +2000,9 @@
       <c r="G36" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H36" s="12"/>
+      <c r="H36" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I36" t="s">
         <v>134</v>
       </c>
@@ -1901,18 +2017,24 @@
       <c r="B37" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="C37" s="12"/>
+      <c r="C37" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D37" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E37" s="15"/>
+      <c r="E37" s="15" t="s">
+        <v>177</v>
+      </c>
       <c r="F37" s="14" t="s">
         <v>108</v>
       </c>
       <c r="G37" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H37" s="12"/>
+      <c r="H37" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I37" t="s">
         <v>136</v>
       </c>
@@ -1927,7 +2049,9 @@
       <c r="B38" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="12"/>
+      <c r="C38" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D38" s="12" t="s">
         <v>75</v>
       </c>
@@ -1940,7 +2064,9 @@
       <c r="G38" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H38" s="12"/>
+      <c r="H38" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I38" t="s">
         <v>175</v>
       </c>
@@ -1955,18 +2081,24 @@
       <c r="B39" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="C39" s="12"/>
+      <c r="C39" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="D39" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="E39" s="15"/>
+      <c r="E39" s="15" t="s">
+        <v>177</v>
+      </c>
       <c r="F39" s="14" t="s">
         <v>108</v>
       </c>
       <c r="G39" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="H39" s="12"/>
+      <c r="H39" s="12" t="s">
+        <v>178</v>
+      </c>
       <c r="I39" t="s">
         <v>147</v>
       </c>

</xml_diff>

<commit_message>
Updated Listeria_monocytogenes_1408MLGX6-3WGS.xlsx, replaced genBankAssembly column, resorted rows by biosample_acc
</commit_message>
<xml_diff>
--- a/datasets/Listeria_monocytogenes_1408MLGX6-3WGS.xlsx
+++ b/datasets/Listeria_monocytogenes_1408MLGX6-3WGS.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\data.biotech.cdc.gov\home\src\datasets\datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\WGS-standards-and-analysis\devel\datasets.git\trunk\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="188">
   <si>
     <t>Organism</t>
   </si>
@@ -364,9 +364,6 @@
     <t>SAMN03093481</t>
   </si>
   <si>
-    <t>CP012021</t>
-  </si>
-  <si>
     <t>1408MLGX6-3WGS</t>
   </si>
   <si>
@@ -578,6 +575,36 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>GCA_001257675.1</t>
+  </si>
+  <si>
+    <t>GCA_001257525.1</t>
+  </si>
+  <si>
+    <t>GCA_001257505.1</t>
+  </si>
+  <si>
+    <t>GCA_001257515.1</t>
+  </si>
+  <si>
+    <t>GCA_001257635.1</t>
+  </si>
+  <si>
+    <t>GCA_001257595.1</t>
+  </si>
+  <si>
+    <t>GCA_001257585.1</t>
+  </si>
+  <si>
+    <t>GCA_001047715.1</t>
+  </si>
+  <si>
+    <t>GCA_001257575.1</t>
+  </si>
+  <si>
+    <t>GCA_001257495.1</t>
   </si>
 </sst>
 </file>
@@ -664,7 +691,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -686,7 +713,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="13"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1014,7 +1040,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1022,7 +1048,7 @@
     <col min="1" max="1" width="18.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.28515625" style="1" customWidth="1"/>
@@ -1037,7 +1063,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1045,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1061,7 +1087,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1116,997 +1142,1000 @@
     </row>
     <row r="9" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>107</v>
+        <v>109</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>178</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>18</v>
+        <v>108</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>108</v>
+        <v>176</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G9" s="12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
       <c r="I9" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="J9" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>20</v>
+        <v>70</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>108</v>
+        <v>69</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G10" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I10" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="J10" t="s">
-        <v>115</v>
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>108</v>
+        <v>71</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G11" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I11" t="s">
-        <v>165</v>
+        <v>133</v>
       </c>
       <c r="J11" t="s">
-        <v>166</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>108</v>
+        <v>35</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G12" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="I12" t="s">
-        <v>149</v>
+        <v>177</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>121</v>
       </c>
       <c r="J12" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>108</v>
+        <v>37</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G13" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I13" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="J13" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>108</v>
+        <v>39</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G14" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I14" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="J14" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>108</v>
+        <v>41</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G15" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I15" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="J15" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>108</v>
+        <v>43</v>
+      </c>
+      <c r="E16" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G16" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H16" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I16" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="J16" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="E17" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>108</v>
+        <v>45</v>
+      </c>
+      <c r="E17" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G17" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I17" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="J17" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>108</v>
+        <v>47</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G18" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H18" s="12" t="s">
-        <v>178</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>122</v>
+        <v>177</v>
+      </c>
+      <c r="I18" t="s">
+        <v>156</v>
       </c>
       <c r="J18" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>108</v>
+        <v>49</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G19" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H19" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I19" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="J19" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="14" t="s">
-        <v>108</v>
+        <v>51</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G20" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I20" t="s">
-        <v>124</v>
+        <v>154</v>
       </c>
       <c r="J20" t="s">
-        <v>125</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="14" t="s">
-        <v>108</v>
+        <v>53</v>
+      </c>
+      <c r="E21" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G21" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I21" t="s">
-        <v>126</v>
+        <v>166</v>
       </c>
       <c r="J21" t="s">
-        <v>127</v>
+        <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F22" s="14" t="s">
-        <v>108</v>
+        <v>55</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G22" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I22" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
       <c r="J22" t="s">
-        <v>129</v>
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>108</v>
+        <v>57</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G23" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I23" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="J23" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>108</v>
+        <v>59</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G24" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I24" t="s">
-        <v>157</v>
+        <v>131</v>
       </c>
       <c r="J24" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>108</v>
+        <v>61</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G25" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I25" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="J25" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
     </row>
     <row r="26" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>108</v>
+        <v>63</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G26" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I26" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="J26" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="12" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>108</v>
+        <v>65</v>
+      </c>
+      <c r="E27" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G27" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H27" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I27" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="J27" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="12" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F28" s="14" t="s">
-        <v>108</v>
+        <v>67</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G28" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I28" t="s">
-        <v>169</v>
-      </c>
-      <c r="J28" t="s">
-        <v>170</v>
+        <v>172</v>
+      </c>
+      <c r="J28" s="15" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>108</v>
+        <v>18</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G29" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>178</v>
+        <v>137</v>
       </c>
       <c r="I29" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="J29" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>108</v>
+        <v>19</v>
+      </c>
+      <c r="E30" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G30" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I30" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="J30" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>108</v>
+        <v>21</v>
+      </c>
+      <c r="E31" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G31" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I31" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="J31" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E32" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F32" s="14" t="s">
-        <v>108</v>
+        <v>23</v>
+      </c>
+      <c r="E32" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G32" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I32" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="J32" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>66</v>
+        <v>26</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>108</v>
+        <v>25</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G33" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I33" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="J33" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
     </row>
     <row r="34" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>68</v>
+        <v>28</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>108</v>
+        <v>27</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G34" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I34" t="s">
-        <v>173</v>
-      </c>
-      <c r="J34" s="16" t="s">
-        <v>174</v>
+        <v>115</v>
+      </c>
+      <c r="J34" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>108</v>
+        <v>29</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G35" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H35" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I35" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="J35" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="E36" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F36" s="14" t="s">
-        <v>108</v>
+        <v>31</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G36" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H36" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I36" t="s">
-        <v>134</v>
+        <v>152</v>
       </c>
       <c r="J36" t="s">
-        <v>135</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="E37" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="F37" s="14" t="s">
-        <v>108</v>
+        <v>33</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G37" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H37" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I37" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="J37" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
     </row>
     <row r="38" spans="1:10" s="7" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="E38" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="F38" s="14" t="s">
-        <v>108</v>
+        <v>73</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G38" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H38" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I38" t="s">
-        <v>175</v>
+        <v>135</v>
       </c>
       <c r="J38" t="s">
-        <v>176</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="F39" s="14" t="s">
-        <v>108</v>
+        <v>75</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="G39" s="12" t="b">
         <v>0</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I39" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="J39" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A9:J39">
+    <sortCondition ref="A8"/>
+  </sortState>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
   </hyperlinks>

</xml_diff>

<commit_message>
updated checksums to reflect nonrefseq loci
</commit_message>
<xml_diff>
--- a/datasets/Listeria_monocytogenes_1408MLGX6-3WGS.xlsx
+++ b/datasets/Listeria_monocytogenes_1408MLGX6-3WGS.xlsx
@@ -12,10 +12,10 @@
     <workbookView xWindow="14235" yWindow="720" windowWidth="32280" windowHeight="24855"/>
   </bookViews>
   <sheets>
-    <sheet name="Lm_strainIds.txt" sheetId="1" r:id="rId1"/>
+    <sheet name="Listeria_monocytogenes_1408MLGX" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="tmpt." localSheetId="0">Lm_strainIds.txt!#REF!</definedName>
+    <definedName name="tmpt." localSheetId="0">Listeria_monocytogenes_1408MLGX!#REF!</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -604,34 +604,34 @@
     <t>GCA_001257495.1</t>
   </si>
   <si>
-    <t>addd50772ddc2bcd22165bf681062f982cb8f9a7b2dbb3a55c46e43ece067565</t>
-  </si>
-  <si>
-    <t>1b749f8c4c8858d549b3cf8a03fce5b108e2a20c735f2fd2dc4044568a285826</t>
-  </si>
-  <si>
-    <t>209d61402a5bae139b77860cf913c473bb7592265175e6c5b1a3bcb69897781c</t>
-  </si>
-  <si>
-    <t>7753439424f11e9dbdfb20b027e937f9ffa5cb71a05a5355d238bcb6f83b89ea</t>
-  </si>
-  <si>
-    <t>f6da330d01631befd8c8433b2d7e2f514e945656dd84024358b6c0c3796735b9</t>
-  </si>
-  <si>
-    <t>36da73e40fc4de2be1ca9e4ae72c3093bc1fd501adf8d7df5ec2abfd2b429944</t>
-  </si>
-  <si>
-    <t>9f4d686ea371e15fabbb70737109c6f6c1f178a9ced3860124655a77e2fac72d</t>
-  </si>
-  <si>
-    <t>39855a345ccbc84bf647d6dfad9b4461b14213343cd3f7c20b2aafe2a837c452</t>
-  </si>
-  <si>
-    <t>7e0feae625305b00bc307425c0bdd4b3deda1255e5772408aae42032472b2c0e</t>
-  </si>
-  <si>
-    <t>9680e4e9063374b0afbd06dce01b1256637d60234d1f6f496ca4de32bc644cad</t>
+    <t>d531614e1b1ba70261a6840d0ca422df90a963d6b9b696d635b8bbcc05cc07af</t>
+  </si>
+  <si>
+    <t>9b926bc0adbea331a0a71f7bf18f6c7a62ebde7dd7a52fabe602ad8b00722c56</t>
+  </si>
+  <si>
+    <t>0543c6777909583f25c96f8942797850af6c7934bdc662b7db680c8d44ed771f</t>
+  </si>
+  <si>
+    <t>ed47ecd6c9bc82592389aafc247a1e6ae7494f0006ce4205861eed548c773085</t>
+  </si>
+  <si>
+    <t>aa128be8a56a30c5d4a55196b341c34fb73664e741723417d573f6f338691f15</t>
+  </si>
+  <si>
+    <t>f203f600a4e8e690c41c1b77611036c8aea96981fef8e85b85c1339cb4a382f2</t>
+  </si>
+  <si>
+    <t>5002591af40007c5da1e31ae2f2a424f596ecd61ae5ab88d2b8ec064436e550a</t>
+  </si>
+  <si>
+    <t>f4c5606eadc763af8e1b284f7eb81ac3414eedc36b5abe4bcf54261e356bc6d4</t>
+  </si>
+  <si>
+    <t>c88f5f94121a2839dd49a09cb87c78b2c506d846765cfca6e62656fe73b393fa</t>
+  </si>
+  <si>
+    <t>5727b8d883ef850863598d63f533f3e53c68be0e8fa82c06c9e81e768ba251a4</t>
   </si>
 </sst>
 </file>
@@ -1067,7 +1067,7 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,7 +1190,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="12" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="I9" t="s">
         <v>145</v>
@@ -1350,7 +1350,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="I14" t="s">
         <v>123</v>
@@ -1542,7 +1542,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I20" t="s">
         <v>153</v>
@@ -1798,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="H28" s="12" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I28" t="s">
         <v>171</v>
@@ -1830,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="I29" t="s">
         <v>161</v>

</xml_diff>